<commit_message>
update import master item
</commit_message>
<xml_diff>
--- a/tests/Import/import_master_item_test.xlsx
+++ b/tests/Import/import_master_item_test.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="37">
   <si>
     <t>No</t>
   </si>
@@ -136,39 +136,6 @@
   </si>
   <si>
     <t>BR013</t>
-  </si>
-  <si>
-    <t>BR014</t>
-  </si>
-  <si>
-    <t>BR015</t>
-  </si>
-  <si>
-    <t>BR016</t>
-  </si>
-  <si>
-    <t>BR017</t>
-  </si>
-  <si>
-    <t>BR018</t>
-  </si>
-  <si>
-    <t>BR019</t>
-  </si>
-  <si>
-    <t>BR020</t>
-  </si>
-  <si>
-    <t>BR021</t>
-  </si>
-  <si>
-    <t>BR022</t>
-  </si>
-  <si>
-    <t>BR023</t>
-  </si>
-  <si>
-    <t>BR024</t>
   </si>
   <si>
     <t>$#$23</t>
@@ -527,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:M27"/>
+  <dimension ref="C3:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -941,10 +908,10 @@
         <v>15</v>
       </c>
       <c r="F14" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="G14" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="H14" t="s">
         <v>11</v>
@@ -1027,12 +994,6 @@
       <c r="C17">
         <v>14</v>
       </c>
-      <c r="D17" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" t="s">
-        <v>15</v>
-      </c>
       <c r="J17" t="s">
         <v>18</v>
       </c>
@@ -1043,356 +1004,6 @@
         <v>1</v>
       </c>
       <c r="M17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C18">
-        <v>15</v>
-      </c>
-      <c r="D18" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" t="s">
-        <v>21</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18">
-        <v>24</v>
-      </c>
-      <c r="H18" t="s">
-        <v>11</v>
-      </c>
-      <c r="I18" t="s">
-        <v>16</v>
-      </c>
-      <c r="J18" t="s">
-        <v>22</v>
-      </c>
-      <c r="K18" t="s">
-        <v>19</v>
-      </c>
-      <c r="L18" t="b">
-        <v>1</v>
-      </c>
-      <c r="M18" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C19">
-        <v>16</v>
-      </c>
-      <c r="D19" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19">
-        <v>2</v>
-      </c>
-      <c r="H19" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" t="s">
-        <v>12</v>
-      </c>
-      <c r="J19" t="s">
-        <v>17</v>
-      </c>
-      <c r="K19" t="s">
-        <v>13</v>
-      </c>
-      <c r="L19" t="b">
-        <v>0</v>
-      </c>
-      <c r="M19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C20">
-        <v>17</v>
-      </c>
-      <c r="D20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E20" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20">
-        <v>10</v>
-      </c>
-      <c r="H20" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" t="s">
-        <v>16</v>
-      </c>
-      <c r="J20" t="s">
-        <v>18</v>
-      </c>
-      <c r="K20" t="s">
-        <v>19</v>
-      </c>
-      <c r="L20" t="b">
-        <v>1</v>
-      </c>
-      <c r="M20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C21">
-        <v>18</v>
-      </c>
-      <c r="D21" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" t="s">
-        <v>21</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <v>24</v>
-      </c>
-      <c r="H21" t="s">
-        <v>11</v>
-      </c>
-      <c r="I21" t="s">
-        <v>16</v>
-      </c>
-      <c r="J21" t="s">
-        <v>22</v>
-      </c>
-      <c r="K21" t="s">
-        <v>19</v>
-      </c>
-      <c r="L21" t="b">
-        <v>1</v>
-      </c>
-      <c r="M21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C22">
-        <v>19</v>
-      </c>
-      <c r="D22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22">
-        <v>2</v>
-      </c>
-      <c r="H22" t="s">
-        <v>11</v>
-      </c>
-      <c r="I22" t="s">
-        <v>12</v>
-      </c>
-      <c r="J22" t="s">
-        <v>17</v>
-      </c>
-      <c r="K22" t="s">
-        <v>13</v>
-      </c>
-      <c r="L22" t="b">
-        <v>0</v>
-      </c>
-      <c r="M22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C23">
-        <v>20</v>
-      </c>
-      <c r="D23" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="G23">
-        <v>10</v>
-      </c>
-      <c r="H23" t="s">
-        <v>11</v>
-      </c>
-      <c r="I23" t="s">
-        <v>16</v>
-      </c>
-      <c r="J23" t="s">
-        <v>18</v>
-      </c>
-      <c r="K23" t="s">
-        <v>19</v>
-      </c>
-      <c r="L23" t="b">
-        <v>1</v>
-      </c>
-      <c r="M23" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C24">
-        <v>21</v>
-      </c>
-      <c r="D24" t="s">
-        <v>42</v>
-      </c>
-      <c r="E24" t="s">
-        <v>21</v>
-      </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-      <c r="G24">
-        <v>24</v>
-      </c>
-      <c r="H24" t="s">
-        <v>11</v>
-      </c>
-      <c r="I24" t="s">
-        <v>16</v>
-      </c>
-      <c r="J24" t="s">
-        <v>22</v>
-      </c>
-      <c r="K24" t="s">
-        <v>19</v>
-      </c>
-      <c r="L24" t="b">
-        <v>1</v>
-      </c>
-      <c r="M24" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C25">
-        <v>22</v>
-      </c>
-      <c r="D25" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-      <c r="G25">
-        <v>2</v>
-      </c>
-      <c r="H25" t="s">
-        <v>11</v>
-      </c>
-      <c r="I25" t="s">
-        <v>12</v>
-      </c>
-      <c r="J25" t="s">
-        <v>17</v>
-      </c>
-      <c r="K25" t="s">
-        <v>13</v>
-      </c>
-      <c r="L25" t="b">
-        <v>0</v>
-      </c>
-      <c r="M25" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C26">
-        <v>23</v>
-      </c>
-      <c r="D26" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26">
-        <v>10</v>
-      </c>
-      <c r="H26" t="s">
-        <v>11</v>
-      </c>
-      <c r="I26" t="s">
-        <v>16</v>
-      </c>
-      <c r="J26" t="s">
-        <v>18</v>
-      </c>
-      <c r="K26" t="s">
-        <v>19</v>
-      </c>
-      <c r="L26" t="b">
-        <v>1</v>
-      </c>
-      <c r="M26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C27">
-        <v>24</v>
-      </c>
-      <c r="D27" t="s">
-        <v>45</v>
-      </c>
-      <c r="E27" t="s">
-        <v>21</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27">
-        <v>24</v>
-      </c>
-      <c r="H27" t="s">
-        <v>11</v>
-      </c>
-      <c r="I27" t="s">
-        <v>16</v>
-      </c>
-      <c r="J27" t="s">
-        <v>22</v>
-      </c>
-      <c r="K27" t="s">
-        <v>19</v>
-      </c>
-      <c r="L27" t="b">
-        <v>1</v>
-      </c>
-      <c r="M27" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>